<commit_message>
Finished up mid term
</commit_message>
<xml_diff>
--- a/Macro Ecnomics/Mid Term.xlsx
+++ b/Macro Ecnomics/Mid Term.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="19155" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Question 1 PP" sheetId="1" r:id="rId1"/>
-    <sheet name="Supply and Demand Schedule" sheetId="2" r:id="rId2"/>
+    <sheet name="Question 52 - Production Graph" sheetId="1" r:id="rId1"/>
+    <sheet name="Question 53 - Supply and Demand" sheetId="2" r:id="rId2"/>
+    <sheet name="Question 54 - Circular Flow" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Chuck Reeves, Production Possibilities Schedule</t>
   </si>
@@ -38,17 +39,59 @@
     <t>F</t>
   </si>
   <si>
-    <t>Data Table</t>
+    <t>Chuck Reeves, Supply and Demand Schedule</t>
   </si>
   <si>
-    <t>Chuck Reeves, Supply and Demand Schedule</t>
+    <t>Price Per Can</t>
+  </si>
+  <si>
+    <t>QTY Smith</t>
+  </si>
+  <si>
+    <t>QTY Morris</t>
+  </si>
+  <si>
+    <t>QTY Lewis</t>
+  </si>
+  <si>
+    <t>Total Market</t>
+  </si>
+  <si>
+    <t>Market Demand Schedule</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>QTY Jones</t>
+  </si>
+  <si>
+    <t>QTY Ryley</t>
+  </si>
+  <si>
+    <t>QTY Shaw</t>
+  </si>
+  <si>
+    <t>Markey Supply Schedule</t>
+  </si>
+  <si>
+    <t>Production Possibilities</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>Tractors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,11 +100,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Verdana"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,26 +219,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,7 +295,7 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>'Question 1 PP'!$B$4:$B$9</c:f>
+              <c:f>'Question 52 - Production Graph'!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -252,7 +322,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Question 1 PP'!$C$4:$C$9</c:f>
+              <c:f>'Question 52 - Production Graph'!$C$5:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -279,13 +349,14 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="50502272"/>
-        <c:axId val="50500736"/>
+        <c:axId val="45017344"/>
+        <c:axId val="45018496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50502272"/>
+        <c:axId val="45017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
@@ -314,12 +385,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50500736"/>
+        <c:crossAx val="45018496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50500736"/>
+        <c:axId val="45018496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +425,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50502272"/>
+        <c:crossAx val="45017344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -363,7 +434,252 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Demand</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="14"/>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.295390268336749E-2"/>
+                  <c:y val="-4.6296296296295877E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> Market</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> Equilibrium: $0.80</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Question 53 - Supply and Demand'!$E$4:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Question 53 - Supply and Demand'!$A$4:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Supply</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Question 53 - Supply and Demand'!$E$12:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Question 53 - Supply and Demand'!$A$12:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="51215744"/>
+        <c:axId val="51234304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="51215744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cans of Soda</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51234304"/>
+        <c:crossesAt val="0.05"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="51234304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.6000000000000002"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Price</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Per Can</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51215744"/>
+        <c:crossesAt val="0.05"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -373,16 +689,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -401,6 +717,843 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="714375"/>
+          <a:ext cx="1790700" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Government</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5153025" y="2324100"/>
+          <a:ext cx="1790700" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Financial</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Institutions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2686050" y="1304925"/>
+          <a:ext cx="1790700" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Businesses</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5133975" y="209550"/>
+          <a:ext cx="1790700" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Households</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28573</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3971926" y="1295399"/>
+          <a:ext cx="819149" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="0"/>
+          <a:endCxn id="7" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="4848226" y="1123950"/>
+          <a:ext cx="828675" cy="1571625"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1631537" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="TextBox 64"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="723900"/>
+          <a:ext cx="1631537" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Labor Land </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>and Capital Management</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="897490" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="TextBox 65"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="1800225"/>
+          <a:ext cx="897490" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Lend Money</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="899477" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="TextBox 66"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2876550" y="2105025"/>
+          <a:ext cx="899477" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Repay Loans</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1296573" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="TextBox 67"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="171450"/>
+          <a:ext cx="1296573" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Goods and Services</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Arrow Connector 72"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="1"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1514476" y="1095375"/>
+          <a:ext cx="1171575" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Straight Arrow Connector 74"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="7" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4800601" y="266700"/>
+          <a:ext cx="904875" cy="1552575"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Arrow Connector 76"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="0"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3905250" y="76201"/>
+          <a:ext cx="904875" cy="1552575"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Straight Arrow Connector 78"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="0"/>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="3167063" y="-1252537"/>
+          <a:ext cx="314325" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="507447" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="TextBox 79"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="1409700"/>
+          <a:ext cx="507447" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Taxes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -689,103 +1842,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C5" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C9" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A9" s="8" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" thickBot="1">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C10" s="8">
         <v>0</v>
       </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -800,30 +2032,309 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C6"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUM(B4:D4)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUM(B12:D12)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUM(B13:D13)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUM(B14:D14)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUM(B15:D15)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUM(B16:D16)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>